<commit_message>
Se ajustan modulos con parametros para generar los informes y comprobantes, se actualiza documentación, se actualiza selenium
</commit_message>
<xml_diff>
--- a/docs/Información técnica EUC Aplicación rechazos depósitos.xlsx
+++ b/docs/Información técnica EUC Aplicación rechazos depósitos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dcastano\Documents\Rechazos\script\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B33A6E6-C5FB-42A9-AA59-1F04972A3185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C4117CC-43B0-455C-A2FC-CB239517ADDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{FC2BEEB0-D51C-4F7D-870D-D77C8593BA45}"/>
+    <workbookView xWindow="-4635" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{FC2BEEB0-D51C-4F7D-870D-D77C8593BA45}"/>
   </bookViews>
   <sheets>
     <sheet name="Diagrama conceptual" sheetId="1" r:id="rId1"/>
@@ -10836,7 +10836,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="494026" y="595964"/>
+          <a:off x="494026" y="591346"/>
           <a:ext cx="1936175" cy="1692461"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
@@ -10891,7 +10891,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="9982" y="958151"/>
+          <a:off x="9982" y="953533"/>
           <a:ext cx="968087" cy="968087"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -10962,7 +10962,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="151755" y="1099924"/>
+        <a:off x="151755" y="1095306"/>
         <a:ext cx="684541" cy="684541"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -10973,7 +10973,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3020329" y="616155"/>
+          <a:off x="3020329" y="611537"/>
           <a:ext cx="2107411" cy="1692461"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
@@ -11041,7 +11041,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3547182" y="870024"/>
+        <a:off x="3547182" y="865406"/>
         <a:ext cx="1027363" cy="1184723"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -11052,7 +11052,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2529711" y="958151"/>
+          <a:off x="2529711" y="953533"/>
           <a:ext cx="968087" cy="968087"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -11114,7 +11114,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2671484" y="1099924"/>
+        <a:off x="2671484" y="1095306"/>
         <a:ext cx="684541" cy="684541"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -11125,7 +11125,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="5332781" y="595964"/>
+          <a:off x="5332781" y="591346"/>
           <a:ext cx="2594824" cy="1692461"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
@@ -11192,7 +11192,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="5981487" y="849833"/>
+        <a:off x="5981487" y="845215"/>
         <a:ext cx="1353757" cy="1184723"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -11203,7 +11203,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="5063159" y="958151"/>
+          <a:off x="5063159" y="953533"/>
           <a:ext cx="968087" cy="968087"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -11265,7 +11265,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="5204932" y="1099924"/>
+        <a:off x="5204932" y="1095306"/>
         <a:ext cx="684541" cy="684541"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -11276,7 +11276,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="8048616" y="595964"/>
+          <a:off x="8048616" y="591346"/>
           <a:ext cx="3483993" cy="1692461"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
@@ -11342,7 +11342,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="8919615" y="849833"/>
+        <a:off x="8919615" y="845215"/>
         <a:ext cx="2020634" cy="1184723"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -11353,7 +11353,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="8036980" y="958151"/>
+          <a:off x="8036980" y="953533"/>
           <a:ext cx="968087" cy="968087"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -11415,7 +11415,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="8178753" y="1099924"/>
+        <a:off x="8178753" y="1095306"/>
         <a:ext cx="684541" cy="684541"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -11426,7 +11426,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="11908393" y="595964"/>
+          <a:off x="11908393" y="591346"/>
           <a:ext cx="2394720" cy="1692461"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
@@ -11492,7 +11492,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="12507073" y="849833"/>
+        <a:off x="12507073" y="845215"/>
         <a:ext cx="1203679" cy="1184723"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -11503,7 +11503,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="11535979" y="942467"/>
+          <a:off x="11535979" y="937849"/>
           <a:ext cx="968087" cy="968087"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -11565,7 +11565,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="11677752" y="1084240"/>
+        <a:off x="11677752" y="1079622"/>
         <a:ext cx="684541" cy="684541"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -11576,7 +11576,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="14845736" y="595964"/>
+          <a:off x="14845736" y="591346"/>
           <a:ext cx="2061039" cy="1692461"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
@@ -11642,7 +11642,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="15360996" y="849833"/>
+        <a:off x="15360996" y="845215"/>
         <a:ext cx="1004756" cy="1184723"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -11653,7 +11653,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="14194387" y="958151"/>
+          <a:off x="14194387" y="953533"/>
           <a:ext cx="968087" cy="968087"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -11715,7 +11715,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="14336160" y="1099924"/>
+        <a:off x="14336160" y="1095306"/>
         <a:ext cx="684541" cy="684541"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -11738,7 +11738,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="444029" y="411979"/>
+          <a:off x="444029" y="408227"/>
           <a:ext cx="1775596" cy="1552094"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
@@ -11793,7 +11793,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="130" y="744127"/>
+          <a:off x="130" y="740375"/>
           <a:ext cx="887798" cy="887798"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -11865,7 +11865,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="130145" y="874142"/>
+        <a:off x="130145" y="870390"/>
         <a:ext cx="627768" cy="627768"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -11876,7 +11876,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2760809" y="430495"/>
+          <a:off x="2760809" y="426743"/>
           <a:ext cx="1932630" cy="1552094"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
@@ -11944,7 +11944,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3243967" y="663309"/>
+        <a:off x="3243967" y="659557"/>
         <a:ext cx="942157" cy="1086466"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -11955,7 +11955,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2310882" y="744127"/>
+          <a:off x="2310882" y="740375"/>
           <a:ext cx="887798" cy="887798"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -12017,7 +12017,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2440897" y="874142"/>
+        <a:off x="2440897" y="870390"/>
         <a:ext cx="627768" cy="627768"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -12028,7 +12028,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4881475" y="411979"/>
+          <a:off x="4881475" y="408227"/>
           <a:ext cx="2379618" cy="1552094"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
@@ -12105,7 +12105,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="5476380" y="644793"/>
+        <a:off x="5476380" y="641041"/>
         <a:ext cx="1241481" cy="1086466"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -12116,7 +12116,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4634215" y="744127"/>
+          <a:off x="4634215" y="740375"/>
           <a:ext cx="887798" cy="887798"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -12178,7 +12178,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4764230" y="874142"/>
+        <a:off x="4764230" y="870390"/>
         <a:ext cx="627768" cy="627768"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -12201,7 +12201,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="517650" y="559862"/>
+          <a:off x="517650" y="555244"/>
           <a:ext cx="2018777" cy="1764665"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
@@ -12256,7 +12256,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="12955" y="937501"/>
+          <a:off x="12955" y="932883"/>
           <a:ext cx="1009388" cy="1009388"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -12328,7 +12328,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="160776" y="1085322"/>
+        <a:off x="160776" y="1080704"/>
         <a:ext cx="713746" cy="713746"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -12339,7 +12339,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3151730" y="580915"/>
+          <a:off x="3151730" y="576297"/>
           <a:ext cx="2197317" cy="1764665"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
@@ -12407,7 +12407,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3701060" y="845615"/>
+        <a:off x="3701060" y="840997"/>
         <a:ext cx="1071192" cy="1235265"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -12418,7 +12418,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2640182" y="937501"/>
+          <a:off x="2640182" y="932883"/>
           <a:ext cx="1009388" cy="1009388"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -12480,7 +12480,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2788003" y="1085322"/>
+        <a:off x="2788003" y="1080704"/>
         <a:ext cx="713746" cy="713746"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -12491,7 +12491,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="5562837" y="559862"/>
+          <a:off x="5562837" y="555244"/>
           <a:ext cx="2705524" cy="1764665"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
@@ -12558,7 +12558,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="6239218" y="824562"/>
+        <a:off x="6239218" y="819944"/>
         <a:ext cx="1411510" cy="1235265"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -12569,7 +12569,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="5281712" y="937501"/>
+          <a:off x="5281712" y="932883"/>
           <a:ext cx="1009388" cy="1009388"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -12631,7 +12631,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="5429533" y="1085322"/>
+        <a:off x="5429533" y="1080704"/>
         <a:ext cx="713746" cy="713746"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -12642,7 +12642,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="8855654" y="559862"/>
+          <a:off x="8855654" y="555244"/>
           <a:ext cx="2105927" cy="1764665"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
@@ -12708,7 +12708,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="9382136" y="824562"/>
+        <a:off x="9382136" y="819944"/>
         <a:ext cx="1026639" cy="1235265"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -12719,7 +12719,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="8080171" y="937501"/>
+          <a:off x="8080171" y="932883"/>
           <a:ext cx="1009388" cy="1009388"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -12781,7 +12781,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="8227992" y="1085322"/>
+        <a:off x="8227992" y="1080704"/>
         <a:ext cx="713746" cy="713746"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -12792,7 +12792,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="11353396" y="559862"/>
+          <a:off x="11353396" y="555244"/>
           <a:ext cx="2496884" cy="1764665"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
@@ -12858,7 +12858,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="11977618" y="824562"/>
+        <a:off x="11977618" y="819944"/>
         <a:ext cx="1255030" cy="1235265"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -12869,7 +12869,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="10965095" y="921149"/>
+          <a:off x="10965095" y="916531"/>
           <a:ext cx="1009388" cy="1009388"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -12931,7 +12931,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="11112916" y="1068970"/>
+        <a:off x="11112916" y="1064352"/>
         <a:ext cx="713746" cy="713746"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -12942,7 +12942,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="14077272" y="559862"/>
+          <a:off x="14077272" y="555244"/>
           <a:ext cx="2826530" cy="1764665"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
@@ -13008,7 +13008,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="14783905" y="824562"/>
+        <a:off x="14783905" y="819944"/>
         <a:ext cx="1502264" cy="1235265"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -13019,7 +13019,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="13736916" y="937501"/>
+          <a:off x="13736916" y="932883"/>
           <a:ext cx="1009388" cy="1009388"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -13081,7 +13081,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="13884737" y="1085322"/>
+        <a:off x="13884737" y="1080704"/>
         <a:ext cx="713746" cy="713746"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -13104,7 +13104,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="472672" y="622346"/>
+          <a:off x="472672" y="617727"/>
           <a:ext cx="1875815" cy="1639698"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
@@ -13159,7 +13159,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3718" y="973241"/>
+          <a:off x="3718" y="968623"/>
           <a:ext cx="937907" cy="937907"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -13231,7 +13231,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="141071" y="1110594"/>
+        <a:off x="141071" y="1105976"/>
         <a:ext cx="663201" cy="663201"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -13242,7 +13242,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2920217" y="641907"/>
+          <a:off x="2920217" y="637289"/>
           <a:ext cx="2041712" cy="1639698"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
@@ -13310,7 +13310,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3430645" y="887862"/>
+        <a:off x="3430645" y="883244"/>
         <a:ext cx="995335" cy="1147788"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -13321,7 +13321,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2444895" y="973241"/>
+          <a:off x="2444895" y="968623"/>
           <a:ext cx="937907" cy="937907"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -13383,7 +13383,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2582248" y="1110594"/>
+        <a:off x="2582248" y="1105976"/>
         <a:ext cx="663201" cy="663201"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -13394,7 +13394,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="5160578" y="622346"/>
+          <a:off x="5160578" y="617727"/>
           <a:ext cx="2513930" cy="1639698"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
@@ -13461,7 +13461,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="5789061" y="868301"/>
+        <a:off x="5789061" y="863682"/>
         <a:ext cx="1311553" cy="1147788"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -13472,7 +13472,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4899362" y="973241"/>
+          <a:off x="4899362" y="968623"/>
           <a:ext cx="937907" cy="937907"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -13534,7 +13534,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="5036715" y="1110594"/>
+        <a:off x="5036715" y="1105976"/>
         <a:ext cx="663201" cy="663201"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -13545,7 +13545,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="7916029" y="622346"/>
+          <a:off x="7916029" y="617727"/>
           <a:ext cx="2565158" cy="1639698"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
@@ -13611,7 +13611,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="8557319" y="868301"/>
+        <a:off x="8557319" y="863682"/>
         <a:ext cx="1349975" cy="1147788"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -13622,7 +13622,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="7499645" y="973241"/>
+          <a:off x="7499645" y="968623"/>
           <a:ext cx="937907" cy="937907"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -13684,7 +13684,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="7636998" y="1110594"/>
+        <a:off x="7636998" y="1105976"/>
         <a:ext cx="663201" cy="663201"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -13707,7 +13707,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="481996" y="606173"/>
+          <a:off x="481996" y="601555"/>
           <a:ext cx="1912818" cy="1672044"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
@@ -13762,7 +13762,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3791" y="963990"/>
+          <a:off x="3791" y="959372"/>
           <a:ext cx="956409" cy="956409"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -13834,7 +13834,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="143854" y="1104053"/>
+        <a:off x="143854" y="1099435"/>
         <a:ext cx="676283" cy="676283"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -13845,7 +13845,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2977822" y="626120"/>
+          <a:off x="2977822" y="621502"/>
           <a:ext cx="2081988" cy="1672044"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
@@ -13913,7 +13913,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3498319" y="876927"/>
+        <a:off x="3498319" y="872309"/>
         <a:ext cx="1014969" cy="1170430"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -13924,7 +13924,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2493124" y="963990"/>
+          <a:off x="2493124" y="959372"/>
           <a:ext cx="956409" cy="956409"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -13986,7 +13986,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2633187" y="1104053"/>
+        <a:off x="2633187" y="1099435"/>
         <a:ext cx="676283" cy="676283"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -13997,7 +13997,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="5262378" y="606173"/>
+          <a:off x="5262378" y="601555"/>
           <a:ext cx="2563520" cy="1672044"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
@@ -14064,7 +14064,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="5903258" y="856980"/>
+        <a:off x="5903258" y="852362"/>
         <a:ext cx="1337425" cy="1170430"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -14075,7 +14075,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4996008" y="963990"/>
+          <a:off x="4996008" y="959372"/>
           <a:ext cx="956409" cy="956409"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -14137,7 +14137,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="5136071" y="1104053"/>
+        <a:off x="5136071" y="1099435"/>
         <a:ext cx="676283" cy="676283"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -14148,7 +14148,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="8072184" y="606173"/>
+          <a:off x="8072184" y="601555"/>
           <a:ext cx="2615760" cy="1672044"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
@@ -14214,7 +14214,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="8726124" y="856980"/>
+        <a:off x="8726124" y="852362"/>
         <a:ext cx="1376605" cy="1170430"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -14225,7 +14225,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="7647586" y="963990"/>
+          <a:off x="7647586" y="959372"/>
           <a:ext cx="956409" cy="956409"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -14287,7 +14287,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="7787649" y="1104053"/>
+        <a:off x="7787649" y="1099435"/>
         <a:ext cx="676283" cy="676283"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -14310,7 +14310,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="444824" y="664360"/>
+          <a:off x="444824" y="660031"/>
           <a:ext cx="1775912" cy="1552371"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
@@ -14365,7 +14365,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="846" y="996568"/>
+          <a:off x="846" y="992238"/>
           <a:ext cx="887956" cy="887956"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -14437,7 +14437,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="130884" y="1126606"/>
+        <a:off x="130884" y="1122276"/>
         <a:ext cx="627880" cy="627880"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -14448,7 +14448,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2954118" y="682880"/>
+          <a:off x="2954118" y="678551"/>
           <a:ext cx="1548773" cy="1552371"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
@@ -14516,7 +14516,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3341311" y="915736"/>
+        <a:off x="3341311" y="911407"/>
         <a:ext cx="755027" cy="1086659"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -14527,7 +14527,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2312010" y="996568"/>
+          <a:off x="2312010" y="992238"/>
           <a:ext cx="887956" cy="887956"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -14589,7 +14589,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2442048" y="1126606"/>
+        <a:off x="2442048" y="1122276"/>
         <a:ext cx="627880" cy="627880"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -14600,7 +14600,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="5038365" y="664360"/>
+          <a:off x="5038365" y="660031"/>
           <a:ext cx="1912374" cy="1552371"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
@@ -14667,7 +14667,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="5516459" y="897216"/>
+        <a:off x="5516459" y="892887"/>
         <a:ext cx="932282" cy="1086659"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -14678,7 +14678,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4557226" y="996568"/>
+          <a:off x="4557226" y="992238"/>
           <a:ext cx="887956" cy="887956"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -14740,7 +14740,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4687264" y="1126606"/>
+        <a:off x="4687264" y="1122276"/>
         <a:ext cx="627880" cy="627880"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -14763,7 +14763,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="433477" y="688416"/>
+          <a:off x="433477" y="684086"/>
           <a:ext cx="1720874" cy="1504260"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
@@ -14818,7 +14818,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3259" y="1010328"/>
+          <a:off x="3259" y="1005998"/>
           <a:ext cx="860437" cy="860437"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -14890,7 +14890,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="129267" y="1136336"/>
+        <a:off x="129267" y="1132006"/>
         <a:ext cx="608421" cy="608421"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -14901,7 +14901,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2865004" y="706362"/>
+          <a:off x="2865004" y="702032"/>
           <a:ext cx="1500774" cy="1504260"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
@@ -14969,7 +14969,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3240198" y="932001"/>
+        <a:off x="3240198" y="927671"/>
         <a:ext cx="731627" cy="1052982"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -14980,7 +14980,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2242796" y="1010328"/>
+          <a:off x="2242796" y="1005998"/>
           <a:ext cx="860437" cy="860437"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -15042,7 +15042,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2368804" y="1136336"/>
+        <a:off x="2368804" y="1132006"/>
         <a:ext cx="608421" cy="608421"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -15053,7 +15053,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="5068635" y="688416"/>
+          <a:off x="5068635" y="684086"/>
           <a:ext cx="1485149" cy="1504260"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
@@ -15120,7 +15120,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="5439923" y="914055"/>
+        <a:off x="5439923" y="909725"/>
         <a:ext cx="724010" cy="1052982"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -15131,7 +15131,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4418429" y="1010328"/>
+          <a:off x="4418429" y="1005998"/>
           <a:ext cx="860437" cy="860437"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -15193,7 +15193,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4544437" y="1136336"/>
+        <a:off x="4544437" y="1132006"/>
         <a:ext cx="608421" cy="608421"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -24766,8 +24766,8 @@
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>666750</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -24783,7 +24783,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="552450" y="152396"/>
-          <a:ext cx="10020300" cy="10737854"/>
+          <a:ext cx="10020300" cy="12757154"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -25109,7 +25109,179 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>3. Ingresar usuario y contraseña de</a:t>
+            <a:t>3. Ingresar contraseña EUC: </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Se mostrará en la pantalla la consola de la EUC en la cual se debe digitar la contraseña de la EUC y luego presionar ENTER.</a:t>
+          </a:r>
+          <a:endParaRPr lang="es-CO" sz="1000" b="0" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="CIBFont Sans" panose="020B0603020202020104" pitchFamily="34" charset="0"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr lvl="0"/>
+          <a:endParaRPr lang="es-CO" sz="1000" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="CIBFont Sans" panose="020B0603020202020104" pitchFamily="34" charset="0"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr lvl="0"/>
+          <a:endParaRPr lang="es-CO" sz="1000" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="CIBFont Sans" panose="020B0603020202020104" pitchFamily="34" charset="0"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr lvl="0"/>
+          <a:endParaRPr lang="es-CO" sz="1000" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="CIBFont Sans" panose="020B0603020202020104" pitchFamily="34" charset="0"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr lvl="0"/>
+          <a:endParaRPr lang="es-CO" sz="1000" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="CIBFont Sans" panose="020B0603020202020104" pitchFamily="34" charset="0"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr lvl="0"/>
+          <a:endParaRPr lang="es-CO" sz="1000" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="CIBFont Sans" panose="020B0603020202020104" pitchFamily="34" charset="0"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr lvl="0"/>
+          <a:endParaRPr lang="es-CO" sz="1000" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="CIBFont Sans" panose="020B0603020202020104" pitchFamily="34" charset="0"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr lvl="0"/>
+          <a:endParaRPr lang="es-CO" sz="1000" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="CIBFont Sans" panose="020B0603020202020104" pitchFamily="34" charset="0"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr lvl="0"/>
+          <a:endParaRPr lang="es-CO" sz="1000" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="CIBFont Sans" panose="020B0603020202020104" pitchFamily="34" charset="0"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr lvl="0"/>
+          <a:endParaRPr lang="es-CO" sz="1000" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="CIBFont Sans" panose="020B0603020202020104" pitchFamily="34" charset="0"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr lvl="0"/>
+          <a:endParaRPr lang="es-CO" sz="1000" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="CIBFont Sans" panose="020B0603020202020104" pitchFamily="34" charset="0"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>4. Ingresar usuario y contraseña de</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="es-CO" sz="1100" b="1" baseline="0">
@@ -25307,7 +25479,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>4. Ingresar usuario y contraseña AS400 NACIONAL: </a:t>
+            <a:t>5. Ingresar usuario y contraseña AS400 NACIONAL: </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="es-CO" sz="1000">
@@ -25509,7 +25681,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>5. </a:t>
+            <a:t>6. </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="es-CO" sz="1100" b="0">
@@ -25642,15 +25814,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>44450</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>88896</xdr:rowOff>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>57146</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>145159</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>115366</xdr:rowOff>
+      <xdr:colOff>119759</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>83616</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -25673,7 +25845,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="806450" y="3587746"/>
+          <a:off x="781050" y="5397496"/>
           <a:ext cx="2386709" cy="1499670"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -25686,15 +25858,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>63500</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>95247</xdr:rowOff>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>63497</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>329307</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>33627</xdr:rowOff>
+      <xdr:colOff>303907</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>1877</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -25717,7 +25889,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="825500" y="5619747"/>
+          <a:off x="800100" y="7429497"/>
           <a:ext cx="2551807" cy="1595730"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -25730,15 +25902,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>120646</xdr:rowOff>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>88896</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>52528</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>98623</xdr:rowOff>
+      <xdr:colOff>27128</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>66873</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -25761,8 +25933,52 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="838200" y="7854946"/>
+          <a:off x="812800" y="9664696"/>
           <a:ext cx="4548328" cy="2740227"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>69846</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>464109</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>27629</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="768350" y="3568696"/>
+          <a:ext cx="5791759" cy="1246833"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -25776,25 +25992,25 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>101600</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>120650</xdr:rowOff>
+          <xdr:rowOff>123825</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>254000</xdr:colOff>
+          <xdr:colOff>200025</xdr:colOff>
           <xdr:row>8</xdr:row>
-          <xdr:rowOff>69850</xdr:rowOff>
+          <xdr:rowOff>85725</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="2051" name="Object 3" hidden="1">
+            <xdr:cNvPr id="2053" name="Object 5" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s2051"/>
+                  <a14:compatExt spid="_x0000_s2053"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3DA79851-B140-4098-DCAA-6162E0AE588C}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB94CC4A-04C5-5352-FA0D-B19D853716A9}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -26196,7 +26412,7 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="E3:L3"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -26229,8 +26445,8 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A2:N26"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="O51" sqref="O51"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -26643,27 +26859,27 @@
   <oleObjects>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Document" dvAspect="DVASPECT_ICON" shapeId="2051" r:id="rId4">
+        <oleObject progId="Document" dvAspect="DVASPECT_ICON" shapeId="2053" r:id="rId4">
           <objectPr defaultSize="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>101600</xdr:colOff>
+                <xdr:colOff>50800</xdr:colOff>
                 <xdr:row>4</xdr:row>
-                <xdr:rowOff>120650</xdr:rowOff>
+                <xdr:rowOff>127000</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>2</xdr:col>
-                <xdr:colOff>254000</xdr:colOff>
+                <xdr:colOff>203200</xdr:colOff>
                 <xdr:row>8</xdr:row>
-                <xdr:rowOff>69850</xdr:rowOff>
+                <xdr:rowOff>88900</xdr:rowOff>
               </to>
             </anchor>
           </objectPr>
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Document" dvAspect="DVASPECT_ICON" shapeId="2051" r:id="rId4"/>
+        <oleObject progId="Document" dvAspect="DVASPECT_ICON" shapeId="2053" r:id="rId4"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </oleObjects>
@@ -26709,6 +26925,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Unknown Document Type" ma:contentTypeID="0x010104" ma:contentTypeVersion="0" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="05d83ceaa0bbd2e3bc716e6e66bd857a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b3d69fe45253d5ff147bb69036b756a7">
     <xsd:element name="properties">
@@ -26822,15 +27047,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{607C42D5-D891-44E3-8066-9D0A014D0A99}">
   <ds:schemaRefs>
@@ -26841,6 +27057,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED3C7D99-D759-49A0-B7E9-7601FF7F33DA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA299655-F653-4CB0-9C1E-18294339D07E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -26854,12 +27078,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED3C7D99-D759-49A0-B7E9-7601FF7F33DA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>